<commit_message>
finish i2c base master board
</commit_message>
<xml_diff>
--- a/Book1(AutoRecovered).xlsx
+++ b/Book1(AutoRecovered).xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pnguy\Documents\GitHub\HyperLoop-Circuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{401F1DFB-5D63-4ECB-9B8F-716C7EA46284}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{62315D61-A216-4CA6-AA16-77B3558389C7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7793" xr2:uid="{2C145C81-39D3-49A9-9F9E-B4BDD6EC8B0F}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7793" xr2:uid="{2C145C81-39D3-49A9-9F9E-B4BDD6EC8B0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -428,7 +427,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>